<commit_message>
remove port, update python-telegram-bot 13.13
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E124"/>
+  <dimension ref="A1:E125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2922,6 +2922,28 @@
         </is>
       </c>
     </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>ddd</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Присутній</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Вино біле</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Приїду на машині</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E5"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
change submit in index.js
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E129"/>
+  <dimension ref="A1:E130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3006,8 +3006,20 @@
           <t>Відсутній</t>
         </is>
       </c>
-      <c r="C129" t="inlineStr"/>
-      <c r="D129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>богдана</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Відсутній</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr"/>
+      <c r="D130" t="inlineStr"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E5"/>

</xml_diff>